<commit_message>
Óra rögzítés funkció teszt
</commit_message>
<xml_diff>
--- a/test/functional/calendar.xlsx
+++ b/test/functional/calendar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Vizsgaremek\Forgalmi-Napl-\test\functional\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{518AAC7F-826A-454D-9777-A719BBB2BB94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E6FD11E-03B6-4AF3-B0B3-3AE09DAAA759}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0B1E403B-62D6-4BAC-8265-82972F2241FE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="47">
   <si>
     <t>Sorszám</t>
   </si>
@@ -207,6 +207,13 @@
 2. A tanár ki választja a "Naptár" oldalt
 3. Naptárnézet megjelenése
 4. Egy "kész", levezetett órára kattint a tanár</t>
+  </si>
+  <si>
+    <t>A végső Km nem lehet kisebb mint a kezdő</t>
+  </si>
+  <si>
+    <t>kezdőKM = "100060"
+végsőKM = "100000"</t>
   </si>
 </sst>
 </file>
@@ -613,10 +620,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A360D597-A89B-4E8E-AB8F-818CBB412531}">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14:F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -829,43 +836,63 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
+        <v>5</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
         <v>6</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B16" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C16" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D16" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E15" s="5" t="s">
+      <c r="E16" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="F15" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
+      <c r="F16" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
         <v>7</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B17" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C17" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D17" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="E17" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="F16" s="3" t="s">
+      <c r="F17" s="3" t="s">
         <v>9</v>
       </c>
     </row>
@@ -976,7 +1003,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>1</v>
       </c>
@@ -1036,7 +1063,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:6" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>4</v>
       </c>

</xml_diff>